<commit_message>
Update Roles and SNMP page
</commit_message>
<xml_diff>
--- a/src/main/java/data/TestCaseData/SomeTestCases.xlsx
+++ b/src/main/java/data/TestCaseData/SomeTestCases.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20145" windowHeight="6045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20145" windowHeight="6045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="Role" sheetId="2" r:id="rId2"/>
+    <sheet name="SNMP" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Key</t>
   </si>
@@ -80,6 +81,18 @@
   </si>
   <si>
     <t>administration|auditor|reporting</t>
+  </si>
+  <si>
+    <t>securityName</t>
+  </si>
+  <si>
+    <t>khang</t>
+  </si>
+  <si>
+    <t>authPro</t>
+  </si>
+  <si>
+    <t>MD5</t>
   </si>
 </sst>
 </file>
@@ -90,7 +103,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -403,10 +416,10 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -457,13 +470,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -503,4 +516,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update SNMP page and fresh write Certificate
</commit_message>
<xml_diff>
--- a/src/main/java/data/TestCaseData/SomeTestCases.xlsx
+++ b/src/main/java/data/TestCaseData/SomeTestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Key</t>
   </si>
@@ -92,7 +92,34 @@
     <t>authPro</t>
   </si>
   <si>
-    <t>MD5</t>
+    <t>authPass</t>
+  </si>
+  <si>
+    <t>privPro</t>
+  </si>
+  <si>
+    <t>privPass</t>
+  </si>
+  <si>
+    <t>DES|AES128|AES192|AES256</t>
+  </si>
+  <si>
+    <t>MD5|SHA</t>
+  </si>
+  <si>
+    <t>SNMPserver</t>
+  </si>
+  <si>
+    <t>SNMPuser</t>
+  </si>
+  <si>
+    <t>SNMPpass</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>100.30.7.130</t>
   </si>
 </sst>
 </file>
@@ -402,7 +429,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -520,28 +547,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run successfully test case SNMP_authPriv
</commit_message>
<xml_diff>
--- a/src/main/java/data/TestCaseData/SomeTestCases.xlsx
+++ b/src/main/java/data/TestCaseData/SomeTestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Key</t>
   </si>
@@ -101,9 +101,6 @@
     <t>privPass</t>
   </si>
   <si>
-    <t>DES|AES128|AES192|AES256</t>
-  </si>
-  <si>
     <t>MD5|SHA</t>
   </si>
   <si>
@@ -119,7 +116,13 @@
     <t>root</t>
   </si>
   <si>
-    <t>100.30.7.130</t>
+    <t>10.30.4.77</t>
+  </si>
+  <si>
+    <t>rootpw</t>
+  </si>
+  <si>
+    <t>DES|AES128</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -582,13 +585,13 @@
         <v>25</v>
       </c>
       <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -596,25 +599,25 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
         <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade test case and xml
</commit_message>
<xml_diff>
--- a/src/main/java/data/TestCaseData/SomeTestCases.xlsx
+++ b/src/main/java/data/TestCaseData/SomeTestCases.xlsx
@@ -86,43 +86,43 @@
     <t>securityName</t>
   </si>
   <si>
+    <t>authPro</t>
+  </si>
+  <si>
+    <t>authPass</t>
+  </si>
+  <si>
+    <t>privPro</t>
+  </si>
+  <si>
+    <t>privPass</t>
+  </si>
+  <si>
+    <t>SNMPserver</t>
+  </si>
+  <si>
+    <t>SNMPuser</t>
+  </si>
+  <si>
+    <t>SNMPpass</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>10.30.4.77</t>
+  </si>
+  <si>
+    <t>rootpw</t>
+  </si>
+  <si>
     <t>khang</t>
   </si>
   <si>
-    <t>authPro</t>
-  </si>
-  <si>
-    <t>authPass</t>
-  </si>
-  <si>
-    <t>privPro</t>
-  </si>
-  <si>
-    <t>privPass</t>
-  </si>
-  <si>
-    <t>MD5|SHA</t>
-  </si>
-  <si>
-    <t>SNMPserver</t>
-  </si>
-  <si>
-    <t>SNMPuser</t>
-  </si>
-  <si>
-    <t>SNMPpass</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>10.30.4.77</t>
-  </si>
-  <si>
-    <t>rootpw</t>
-  </si>
-  <si>
-    <t>DES|AES128</t>
+    <t>MD5</t>
+  </si>
+  <si>
+    <t>DES</t>
   </si>
 </sst>
 </file>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -573,33 +573,33 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
         <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -611,13 +611,13 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgrade test case check tomcat version, EXPPORTAL-2969, EPMServersPage
</commit_message>
<xml_diff>
--- a/src/main/java/data/TestCaseData/SomeTestCases.xlsx
+++ b/src/main/java/data/TestCaseData/SomeTestCases.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20145" windowHeight="6045" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20145" windowHeight="6045" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="Role" sheetId="2" r:id="rId2"/>
     <sheet name="SNMP" sheetId="3" r:id="rId3"/>
+    <sheet name="Alarm_Code" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Key</t>
   </si>
@@ -116,13 +117,31 @@
     <t>rootpw</t>
   </si>
   <si>
-    <t>khang</t>
-  </si>
-  <si>
     <t>MD5</t>
   </si>
   <si>
     <t>DES</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>AlarmCode</t>
+  </si>
+  <si>
+    <t>TrapID</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>QADMN01005</t>
+  </si>
+  <si>
+    <t>VerifyMessage</t>
+  </si>
+  <si>
+    <t>The information that you entered has been saved.</t>
   </si>
 </sst>
 </file>
@@ -552,18 +571,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -596,16 +615,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -618,6 +637,55 @@
       </c>
       <c r="H2" t="s">
         <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>17126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade test case EXPPORTAL-2969, SNMP_authPriv
</commit_message>
<xml_diff>
--- a/src/main/java/data/TestCaseData/SomeTestCases.xlsx
+++ b/src/main/java/data/TestCaseData/SomeTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20145" windowHeight="6045" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20145" windowHeight="6045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Key</t>
   </si>
@@ -138,10 +138,16 @@
     <t>QADMN01005</t>
   </si>
   <si>
-    <t>VerifyMessage</t>
-  </si>
-  <si>
     <t>The information that you entered has been saved.</t>
+  </si>
+  <si>
+    <t>verify</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>"17126"</t>
   </si>
 </sst>
 </file>
@@ -177,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,10 +576,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -587,7 +594,7 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -612,8 +619,14 @@
       <c r="H1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -637,6 +650,12 @@
       </c>
       <c r="H2" t="s">
         <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -646,21 +665,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -668,27 +686,22 @@
         <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2">
-        <v>17126</v>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>